<commit_message>
Added some results of the tests done
</commit_message>
<xml_diff>
--- a/TP4/Results.xlsx
+++ b/TP4/Results.xlsx
@@ -163,7 +163,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -213,7 +213,9 @@
       <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="2" t="n">
+        <v>1311</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
@@ -231,7 +233,9 @@
       <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="2" t="n">
+        <v>320.7</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
@@ -249,7 +253,9 @@
       <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2" t="n">
+        <v>78.52</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
@@ -267,7 +273,9 @@
       <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2" t="n">
+        <v>101.5</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
@@ -285,7 +293,9 @@
       <c r="E6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2" t="n">
+        <v>0.008772</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
@@ -303,7 +313,9 @@
       <c r="E7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="2" t="n">
+        <v>6.235</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
@@ -321,7 +333,9 @@
       <c r="E8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="2" t="n">
+        <v>5.625</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">

</xml_diff>

<commit_message>
More test results and images
</commit_message>
<xml_diff>
--- a/TP4/Results.xlsx
+++ b/TP4/Results.xlsx
@@ -163,7 +163,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -453,6 +453,9 @@
       <c r="E14" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F14" s="1" t="n">
+        <v>0.0002281</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
@@ -469,6 +472,9 @@
       </c>
       <c r="E15" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>0.3861</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>